<commit_message>
mise a jour du 27-05-2021
</commit_message>
<xml_diff>
--- a/Complaints_internet/dataset_internet.xlsx
+++ b/Complaints_internet/dataset_internet.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y38"/>
+  <dimension ref="A1:Y78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="Y24" sqref="Y24"/>
@@ -5103,6 +5103,4899 @@
         </is>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>624042741830054</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>C54F7C3A0A1BE70B738274D833C1DC5A</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>237668608391</t>
+        </is>
+      </c>
+      <c r="S39" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="T39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V39" t="inlineStr">
+        <is>
+          <t>n-mms</t>
+        </is>
+      </c>
+      <c r="W39" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X39" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>624042741830054</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>C54F7C3A0A1BE70B738274D833C1DC5A</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>237668608391</t>
+        </is>
+      </c>
+      <c r="S40" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="T40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V40" t="inlineStr">
+        <is>
+          <t>n-mms</t>
+        </is>
+      </c>
+      <c r="W40" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X40" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>6FC8FE718D30FECCB528C3E2C803125F</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="T41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V41" t="inlineStr">
+        <is>
+          <t>n-internet</t>
+        </is>
+      </c>
+      <c r="W41" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="X41" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>6FC8FE718D30FECCB528C3E2C803125F</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="T42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V42" t="inlineStr">
+        <is>
+          <t>n-internet</t>
+        </is>
+      </c>
+      <c r="W42" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="X42" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="V43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="W43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X43" t="inlineStr">
+        <is>
+          <t>searchResponse:requestID=af2fdfdf-204f-41f2-8105-6aa062c582d5, errorCode=32, errorMessage= error result (32); matchedDN = dc=MSISDN,DC=C-NTDB,entries:
+END OF SEARCH ENTRIES.,</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>6FC8FE718D30FECCB528C3E2C803125F</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="S44" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="T44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V44" t="inlineStr">
+        <is>
+          <t>n-internet</t>
+        </is>
+      </c>
+      <c r="W44" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="X44" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="V45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="W45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X45" t="inlineStr">
+        <is>
+          <t>searchResponse:requestID=08198b8d-24c8-4a63-b38d-1e451ea993ff, errorCode=32, errorMessage= error result (32); matchedDN = dc=MSISDN,DC=C-NTDB,entries:
+END OF SEARCH ENTRIES.,</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="V46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="W46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X46" t="inlineStr">
+        <is>
+          <t>searchResponse:requestID=2dba31ec-e74b-444a-94ee-ecfd3626af46, errorCode=32, errorMessage= error result (32); matchedDN = dc=MSISDN,DC=C-NTDB,entries:
+END OF SEARCH ENTRIES.,</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>6FC8FE718D30FECCB528C3E2C803125F</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="T47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V47" t="inlineStr">
+        <is>
+          <t>n-internet</t>
+        </is>
+      </c>
+      <c r="W47" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="X47" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="V48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="W48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X48" t="inlineStr">
+        <is>
+          <t>searchResponse:requestID=8f0406ab-f008-4178-a246-9db36597aa34, errorCode=32, errorMessage= error result (32); matchedDN = dc=MSISDN,DC=C-NTDB,entries:
+END OF SEARCH ENTRIES.,</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="U49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="V49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="W49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X49" t="inlineStr">
+        <is>
+          <t>searchResponse:requestID=0f09bb9d-7f26-43f7-8c97-4d8906f8f08a, errorCode=32, errorMessage= error result (32); matchedDN = dc=MSISDN,DC=C-NTDB,entries:
+END OF SEARCH ENTRIES.,</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="V50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="W50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X50" t="inlineStr">
+        <is>
+          <t>searchResponse:requestID=77e1a11e-9680-4768-b5d1-2ddc78ff758c, errorCode=32, errorMessage= error result (32); matchedDN = dc=MSISDN,DC=C-NTDB,entries:
+END OF SEARCH ENTRIES.,</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="U51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="V51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="W51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X51" t="inlineStr">
+        <is>
+          <t>searchResponse:requestID=d4219132-0e77-44ff-b8c2-88b0ed4baef0, errorCode=32, errorMessage= error result (32); matchedDN = dc=MSISDN,DC=C-NTDB,entries:
+END OF SEARCH ENTRIES.,</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="U52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="V52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="W52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X52" t="inlineStr">
+        <is>
+          <t>searchResponse:requestID=debae303-9f90-480d-b13a-50e6b04f8be8, errorCode=32, errorMessage= error result (32); matchedDN = dc=MSISDN,DC=C-NTDB,entries:
+END OF SEARCH ENTRIES.,</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>6FC8FE718D30FECCB528C3E2C803125F</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="T53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V53" t="inlineStr">
+        <is>
+          <t>n-internet</t>
+        </is>
+      </c>
+      <c r="W53" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="X53" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>6FC8FE718D30FECCB528C3E2C803125F</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="S54" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="T54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U54" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V54" t="inlineStr">
+        <is>
+          <t>n-internet</t>
+        </is>
+      </c>
+      <c r="W54" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="X54" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>6FC8FE718D30FECCB528C3E2C803125F</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="T55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U55" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V55" t="inlineStr">
+        <is>
+          <t>n-internet</t>
+        </is>
+      </c>
+      <c r="W55" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="X55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>6FC8FE718D30FECCB528C3E2C803125F</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="T56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U56" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V56" t="inlineStr">
+        <is>
+          <t>n-internet</t>
+        </is>
+      </c>
+      <c r="W56" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="X56" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>6FC8FE718D30FECCB528C3E2C803125F</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="T57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U57" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V57" t="inlineStr">
+        <is>
+          <t>n-internet</t>
+        </is>
+      </c>
+      <c r="W57" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="X57" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="U58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="V58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="W58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X58" t="inlineStr">
+        <is>
+          <t>searchResponse:requestID=3604fe5f-b235-4ab0-ab29-b7bb39779e67, errorCode=32, errorMessage= error result (32); matchedDN = dc=MSISDN,DC=C-NTDB,entries:
+END OF SEARCH ENTRIES.,</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>624042719604575</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>CADE49F922E4C59399D4BA0ED1F3EEA2</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="R59" t="inlineStr">
+        <is>
+          <t>237667066226</t>
+        </is>
+      </c>
+      <c r="S59" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="T59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U59" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V59" t="inlineStr">
+        <is>
+          <t>b-connect</t>
+        </is>
+      </c>
+      <c r="W59" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X59" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>6FC8FE718D30FECCB528C3E2C803125F</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P60" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="S60" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="T60" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U60" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V60" t="inlineStr">
+        <is>
+          <t>n-internet</t>
+        </is>
+      </c>
+      <c r="W60" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="X60" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>6FC8FE718D30FECCB528C3E2C803125F</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R61" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="S61" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="T61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U61" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V61" t="inlineStr">
+        <is>
+          <t>n-internet</t>
+        </is>
+      </c>
+      <c r="W61" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="X61" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>6FC8FE718D30FECCB528C3E2C803125F</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R62" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="S62" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="T62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U62" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V62" t="inlineStr">
+        <is>
+          <t>n-internet</t>
+        </is>
+      </c>
+      <c r="W62" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="X62" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="U63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="V63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="W63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X63" t="inlineStr">
+        <is>
+          <t>searchResponse:requestID=bd747a3d-d995-4213-96fb-2d0f0757b21b, errorCode=32, errorMessage= error result (32); matchedDN = dc=MSISDN,DC=C-NTDB,entries:
+END OF SEARCH ENTRIES.,</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>624042719604575</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>CADE49F922E4C59399D4BA0ED1F3EEA2</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="R64" t="inlineStr">
+        <is>
+          <t>237667066226</t>
+        </is>
+      </c>
+      <c r="S64" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="T64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U64" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V64" t="inlineStr">
+        <is>
+          <t>b-connect</t>
+        </is>
+      </c>
+      <c r="W64" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X64" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="U65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="V65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="W65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X65" t="inlineStr">
+        <is>
+          <t>searchResponse:requestID=ed968157-1279-4ec4-adba-1af828455fd4, errorCode=32, errorMessage= error result (32); matchedDN = dc=MSISDN,DC=C-NTDB,entries:
+END OF SEARCH ENTRIES.,</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>624042741830054</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>C54F7C3A0A1BE70B738274D833C1DC5A</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R66" t="inlineStr">
+        <is>
+          <t>237668608391</t>
+        </is>
+      </c>
+      <c r="S66" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="T66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U66" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V66" t="inlineStr">
+        <is>
+          <t>n-mms</t>
+        </is>
+      </c>
+      <c r="W66" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X66" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>6FC8FE718D30FECCB528C3E2C803125F</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R67" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="S67" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="T67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U67" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V67" t="inlineStr">
+        <is>
+          <t>n-internet</t>
+        </is>
+      </c>
+      <c r="W67" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="X67" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>624042747827156</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>6FC8FE718D30FECCB528C3E2C803125F</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q68" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R68" t="inlineStr">
+        <is>
+          <t>237669595858</t>
+        </is>
+      </c>
+      <c r="S68" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="T68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U68" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V68" t="inlineStr">
+        <is>
+          <t>n-internet</t>
+        </is>
+      </c>
+      <c r="W68" t="inlineStr">
+        <is>
+          <t>8630780379935655</t>
+        </is>
+      </c>
+      <c r="X68" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>624042719604575</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>CADE49F922E4C59399D4BA0ED1F3EEA2</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="R69" t="inlineStr">
+        <is>
+          <t>237667066226</t>
+        </is>
+      </c>
+      <c r="S69" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="T69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U69" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V69" t="inlineStr">
+        <is>
+          <t>b-connect</t>
+        </is>
+      </c>
+      <c r="W69" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X69" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="U70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="V70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="W70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X70" t="inlineStr">
+        <is>
+          <t>searchResponse:requestID=10f8eb9c-f017-4b2d-bcdd-0cca42f33200, errorCode=32, errorMessage= error result (32); matchedDN = dc=MSISDN,DC=C-NTDB,entries:
+END OF SEARCH ENTRIES.,</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>624042741830054</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>C54F7C3A0A1BE70B738274D833C1DC5A</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R71" t="inlineStr">
+        <is>
+          <t>237668608391</t>
+        </is>
+      </c>
+      <c r="S71" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="T71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U71" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V71" t="inlineStr">
+        <is>
+          <t>n-mms</t>
+        </is>
+      </c>
+      <c r="W71" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X71" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>624042741830088</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>E115120ECC5F6A23514465853CA96D1F</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R72" t="inlineStr">
+        <is>
+          <t>237668608440</t>
+        </is>
+      </c>
+      <c r="S72" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="T72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U72" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V72" t="inlineStr">
+        <is>
+          <t>n-mms</t>
+        </is>
+      </c>
+      <c r="W72" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X72" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>624042741829977</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>63A5D4591DB73211740092C97971137F</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="R73" t="inlineStr">
+        <is>
+          <t>237668608271</t>
+        </is>
+      </c>
+      <c r="S73" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="T73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U73" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V73" t="inlineStr">
+        <is>
+          <t>n-mms</t>
+        </is>
+      </c>
+      <c r="W73" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X73" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>624042741769353</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>CE31AF366198601FC679CE7E8EC03C05</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="R74" t="inlineStr">
+        <is>
+          <t>237667720297</t>
+        </is>
+      </c>
+      <c r="S74" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="T74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U74" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V74" t="inlineStr">
+        <is>
+          <t>n-mms</t>
+        </is>
+      </c>
+      <c r="W74" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X74" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>624042741769353</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>CE31AF366198601FC679CE7E8EC03C05</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="R75" t="inlineStr">
+        <is>
+          <t>237667720297</t>
+        </is>
+      </c>
+      <c r="S75" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="T75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U75" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V75" t="inlineStr">
+        <is>
+          <t>n-mms</t>
+        </is>
+      </c>
+      <c r="W75" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X75" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>624042741769353</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>CE31AF366198601FC679CE7E8EC03C05</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="R76" t="inlineStr">
+        <is>
+          <t>237667720297</t>
+        </is>
+      </c>
+      <c r="S76" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="T76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U76" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V76" t="inlineStr">
+        <is>
+          <t>n-mms</t>
+        </is>
+      </c>
+      <c r="W76" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X76" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="U77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="V77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="W77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X77" t="inlineStr">
+        <is>
+          <t>searchResponse:requestID=4f7263e4-d518-48c2-89be-b64f325c32e4, errorCode=34, errorMessage= error result (34),entries:
+END OF SEARCH ENTRIES.,</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>624042741830054</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>C54F7C3A0A1BE70B738274D833C1DC5A</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q78" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R78" t="inlineStr">
+        <is>
+          <t>237668608391</t>
+        </is>
+      </c>
+      <c r="S78" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="T78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U78" t="inlineStr">
+        <is>
+          <t>QoS-R7</t>
+        </is>
+      </c>
+      <c r="V78" t="inlineStr">
+        <is>
+          <t>n-mms</t>
+        </is>
+      </c>
+      <c r="W78" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="X78" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>